<commit_message>
Added EMNIST to writeup
</commit_message>
<xml_diff>
--- a/EPQ Writeups/Testing.xlsx
+++ b/EPQ Writeups/Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samlaister/Documents/GitHub/NEA-Neural-Network/EPQ Writeups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6EE87F-1940-E449-B492-2347FB852028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183F22A3-48AA-9F45-B6F2-BF435B1002AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{21185252-FFAA-4D03-8DE8-AE2408007027}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
   <si>
     <t>Target Number</t>
   </si>
@@ -81,6 +81,96 @@
   </si>
   <si>
     <t>76-100%</t>
+  </si>
+  <si>
+    <t>MNIST</t>
+  </si>
+  <si>
+    <t>EMNIST</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Out of 3 guesses</t>
+  </si>
+  <si>
+    <t>Test of 100 random samples</t>
   </si>
 </sst>
 </file>
@@ -160,7 +250,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -383,11 +473,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -410,6 +633,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -428,9 +654,31 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,10 +993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C791DB-56EF-4469-B0C2-D327025D026F}">
-  <dimension ref="B2:L20"/>
+  <dimension ref="A2:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -766,25 +1014,29 @@
     <col min="12" max="12" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+    <row r="2" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="H3" s="25" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="H3" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="27"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="30"/>
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="38"/>
+      <c r="B4" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -811,8 +1063,9 @@
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="16">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="38"/>
+      <c r="B5" s="41">
         <v>0</v>
       </c>
       <c r="C5" s="1">
@@ -840,8 +1093,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="17">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="38"/>
+      <c r="B6" s="42">
         <v>1</v>
       </c>
       <c r="C6" s="2">
@@ -869,8 +1123,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="17">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="38"/>
+      <c r="B7" s="42">
         <v>2</v>
       </c>
       <c r="C7" s="2">
@@ -893,13 +1148,14 @@
       <c r="I7" s="2">
         <v>6</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="22">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="17">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="38"/>
+      <c r="B8" s="42">
         <v>3</v>
       </c>
       <c r="C8" s="2">
@@ -927,8 +1183,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="17">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="38"/>
+      <c r="B9" s="42">
         <v>4</v>
       </c>
       <c r="C9" s="2">
@@ -956,8 +1213,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="17">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="38"/>
+      <c r="B10" s="42">
         <v>5</v>
       </c>
       <c r="C10" s="2">
@@ -980,13 +1238,14 @@
       <c r="I10" s="2">
         <v>4</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="22">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="17">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="38"/>
+      <c r="B11" s="42">
         <v>6</v>
       </c>
       <c r="C11" s="2">
@@ -1009,13 +1268,14 @@
       <c r="I11" s="2">
         <v>5</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="23">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="17">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="38"/>
+      <c r="B12" s="42">
         <v>7</v>
       </c>
       <c r="C12" s="2">
@@ -1038,13 +1298,14 @@
       <c r="I12" s="2">
         <v>5</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="23">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="17">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="38"/>
+      <c r="B13" s="42">
         <v>8</v>
       </c>
       <c r="C13" s="2">
@@ -1067,13 +1328,14 @@
       <c r="I13" s="2">
         <v>5</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="23">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="18">
+    <row r="14" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="43">
         <v>9</v>
       </c>
       <c r="C14" s="3">
@@ -1096,24 +1358,28 @@
       <c r="I14" s="3">
         <v>6</v>
       </c>
-      <c r="J14" s="30">
+      <c r="J14" s="24">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="22" t="s">
+    <row r="15" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+    </row>
+    <row r="16" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="H16" s="22" t="s">
+      <c r="C16" s="27"/>
+      <c r="H16" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="24"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="5" t="s">
+      <c r="I16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="38"/>
+      <c r="B17" s="44" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1126,8 +1392,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="5" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="38"/>
+      <c r="B18" s="44" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1140,8 +1407,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="38"/>
+      <c r="B19" s="44" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1154,8 +1422,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+    <row r="20" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="39"/>
+      <c r="B20" s="45" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1168,13 +1437,942 @@
         <v>10</v>
       </c>
     </row>
+    <row r="23" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27"/>
+      <c r="H24" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24" s="29"/>
+      <c r="J24" s="30"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="38"/>
+      <c r="B25" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="38"/>
+      <c r="B26" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <f>C26-D26</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="15">
+        <f>ROUND(D26/C26*100, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="1">
+        <v>2</v>
+      </c>
+      <c r="J26" s="21">
+        <f>I26/10*100</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="38"/>
+      <c r="B27" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="2">
+        <v>6</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2">
+        <f>C27-D27</f>
+        <v>4</v>
+      </c>
+      <c r="F27" s="15">
+        <f t="shared" ref="F27:F50" si="3">ROUND(D27/C27*100, 1)</f>
+        <v>33.299999999999997</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="21">
+        <f t="shared" ref="J27:J51" si="4">I27/10*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="38"/>
+      <c r="B28" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="2">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" ref="E28:E51" si="5">C28-D28</f>
+        <v>3</v>
+      </c>
+      <c r="F28" s="15">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="38"/>
+      <c r="B29" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F29" s="15">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="38"/>
+      <c r="B30" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F30" s="15">
+        <f t="shared" si="3"/>
+        <v>33.299999999999997</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1</v>
+      </c>
+      <c r="J30" s="21">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="38"/>
+      <c r="B31" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="F31" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="2">
+        <v>2</v>
+      </c>
+      <c r="J31" s="21">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="38"/>
+      <c r="B32" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F32" s="15">
+        <f t="shared" si="3"/>
+        <v>33.299999999999997</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="2">
+        <v>3</v>
+      </c>
+      <c r="J32" s="21">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="38"/>
+      <c r="B33" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="2">
+        <v>6</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="F33" s="15">
+        <f t="shared" si="3"/>
+        <v>33.299999999999997</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" s="2">
+        <v>1</v>
+      </c>
+      <c r="J33" s="21">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="38"/>
+      <c r="B34" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="2">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F34" s="15">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="38"/>
+      <c r="B35" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="2">
+        <v>4</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F35" s="15">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="38"/>
+      <c r="B36" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="2">
+        <v>4</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="F36" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="2">
+        <v>2</v>
+      </c>
+      <c r="J36" s="21">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="38"/>
+      <c r="B37" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="2">
+        <v>5</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="F37" s="15">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="I37" s="2">
+        <v>3</v>
+      </c>
+      <c r="J37" s="21">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="38"/>
+      <c r="B38" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="2">
+        <v>5</v>
+      </c>
+      <c r="D38" s="2">
+        <v>5</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="15">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="2">
+        <v>3</v>
+      </c>
+      <c r="J38" s="21">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="38"/>
+      <c r="B39" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="15">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="H39" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I39" s="2">
+        <v>1</v>
+      </c>
+      <c r="J39" s="21">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="38"/>
+      <c r="B40" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="2">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F40" s="15">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="H40" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1</v>
+      </c>
+      <c r="J40" s="21">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="38"/>
+      <c r="B41" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F41" s="15">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="I41" s="2">
+        <v>0</v>
+      </c>
+      <c r="J41" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="38"/>
+      <c r="B42" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="2">
+        <v>4</v>
+      </c>
+      <c r="D42" s="2">
+        <v>3</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F42" s="15">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="H42" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0</v>
+      </c>
+      <c r="J42" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="38"/>
+      <c r="B43" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="15">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="H43" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0</v>
+      </c>
+      <c r="J43" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="38"/>
+      <c r="B44" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="2">
+        <v>6</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="F44" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0</v>
+      </c>
+      <c r="J44" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="38"/>
+      <c r="B45" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="2">
+        <v>7</v>
+      </c>
+      <c r="D45" s="2">
+        <v>4</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="F45" s="15">
+        <f t="shared" si="3"/>
+        <v>57.1</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="I45" s="2">
+        <v>1</v>
+      </c>
+      <c r="J45" s="21">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="38"/>
+      <c r="B46" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F46" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H46" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I46" s="2">
+        <v>1</v>
+      </c>
+      <c r="J46" s="21">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="38"/>
+      <c r="B47" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="2">
+        <v>4</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="F47" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H47" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0</v>
+      </c>
+      <c r="J47" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="38"/>
+      <c r="B48" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="2">
+        <v>6</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="F48" s="15">
+        <f t="shared" si="3"/>
+        <v>16.7</v>
+      </c>
+      <c r="H48" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="I48" s="2">
+        <v>2</v>
+      </c>
+      <c r="J48" s="21">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="38"/>
+      <c r="B49" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="2">
+        <v>2</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F49" s="15">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="H49" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I49" s="2">
+        <v>0</v>
+      </c>
+      <c r="J49" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="38"/>
+      <c r="B50" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="2">
+        <v>3</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="F50" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H50" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I50" s="2">
+        <v>0</v>
+      </c>
+      <c r="J50" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="38"/>
+      <c r="B51" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="3">
+        <v>4</v>
+      </c>
+      <c r="D51" s="3">
+        <v>4</v>
+      </c>
+      <c r="E51" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="46">
+        <f>ROUND(D51/C51*100, 1)</f>
+        <v>100</v>
+      </c>
+      <c r="H51" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="I51" s="3">
+        <v>3</v>
+      </c>
+      <c r="J51" s="47">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="38"/>
+    </row>
+    <row r="53" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="38"/>
+      <c r="B53" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="27"/>
+      <c r="H53" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I53" s="27"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="38"/>
+      <c r="B54" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="38"/>
+      <c r="B55" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="38"/>
+      <c r="B56" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="39"/>
+      <c r="B57" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="10">
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="A24:A57"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="H3:J3"/>
+    <mergeCell ref="A3:A20"/>
   </mergeCells>
+  <conditionalFormatting sqref="F26:F51">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J26:J51">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>